<commit_message>
Added code for finding part characteristics
</commit_message>
<xml_diff>
--- a/BOMs/BOM_1.xlsx
+++ b/BOMs/BOM_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsheb\PushPin\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2664B32A-2C55-4E23-9774-DACD1656BB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA1DBA1-B6E5-4CF1-A2F1-E6742400C1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D334EC07-162C-4D88-B7CF-9AC4FDBCC14E}"/>
   </bookViews>
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1241FFF6-AC8B-4D12-B7BD-2C9C2623FE2A}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,223 +560,223 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="D2" s="2">
-        <v>0.21</v>
+        <v>0.31</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="D3" s="2">
-        <v>0.38</v>
+        <v>0.2</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2">
-        <v>0.31</v>
+        <v>0.1</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="2">
-        <v>0.1</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2">
-        <v>0.1</v>
+        <v>0.24</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2">
-        <v>0.56000000000000005</v>
+        <v>0.1</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2">
-        <v>0.24</v>
+        <v>0.1</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="D10" s="2">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>0.1</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C12" s="2">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D12" s="2">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2">
-        <v>0.14000000000000001</v>
+        <v>0.21</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2">
         <v>36</v>
       </c>
-      <c r="C14" s="2">
-        <v>86</v>
-      </c>
       <c r="D14" s="2">
-        <v>0.1</v>
+        <v>0.38</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logic for determining the resistances
</commit_message>
<xml_diff>
--- a/BOMs/BOM_1.xlsx
+++ b/BOMs/BOM_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsheb\PushPin\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA1DBA1-B6E5-4CF1-A2F1-E6742400C1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA42C6E-DAF4-4EC3-9993-86943B101FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D334EC07-162C-4D88-B7CF-9AC4FDBCC14E}"/>
+    <workbookView xWindow="5160" yWindow="6576" windowWidth="17280" windowHeight="9960" xr2:uid="{D334EC07-162C-4D88-B7CF-9AC4FDBCC14E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Part Number</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Susumu</t>
   </si>
   <si>
-    <t>RR0816P-721-F-M</t>
-  </si>
-  <si>
     <t>R162-R269</t>
   </si>
   <si>
@@ -165,6 +162,15 @@
   </si>
   <si>
     <t>R1-R43</t>
+  </si>
+  <si>
+    <t>RR0816P-721-D</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>RK73H1ETTPE1R13F</t>
   </si>
 </sst>
 </file>
@@ -522,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1241FFF6-AC8B-4D12-B7BD-2C9C2623FE2A}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,10 +555,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -563,7 +569,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2">
         <v>84</v>
@@ -628,10 +634,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
         <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -640,7 +646,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -696,10 +702,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
       </c>
       <c r="C10" s="2">
         <v>108</v>
@@ -713,10 +719,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -725,15 +731,15 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
       </c>
       <c r="C12" s="2">
         <v>86</v>
@@ -742,7 +748,7 @@
         <v>0.1</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -777,6 +783,14 @@
       </c>
       <c r="G14" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logic for determining the capacitance
</commit_message>
<xml_diff>
--- a/BOMs/BOM_1.xlsx
+++ b/BOMs/BOM_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsheb\PushPin\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA42C6E-DAF4-4EC3-9993-86943B101FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A00C3E6-521A-4469-A267-81CFF47E15F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="6576" windowWidth="17280" windowHeight="9960" xr2:uid="{D334EC07-162C-4D88-B7CF-9AC4FDBCC14E}"/>
+    <workbookView xWindow="4116" yWindow="156" windowWidth="17280" windowHeight="9960" xr2:uid="{D334EC07-162C-4D88-B7CF-9AC4FDBCC14E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>KAM15GS71C563CU</t>
-  </si>
-  <si>
     <t>Manufactuer</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>RK73H1ETTPE1R13F</t>
+  </si>
+  <si>
+    <t>KAM15GS71C568CU</t>
   </si>
 </sst>
 </file>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1241FFF6-AC8B-4D12-B7BD-2C9C2623FE2A}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,21 +555,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2">
         <v>84</v>
@@ -578,15 +578,15 @@
         <v>0.31</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="2">
         <v>112</v>
@@ -595,15 +595,15 @@
         <v>0.2</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
@@ -612,15 +612,15 @@
         <v>0.1</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2">
         <v>100</v>
@@ -629,15 +629,15 @@
         <v>0.1</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -646,15 +646,15 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="2">
         <v>14</v>
@@ -663,15 +663,15 @@
         <v>0.24</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2">
         <v>25</v>
@@ -680,15 +680,15 @@
         <v>0.1</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2">
         <v>21</v>
@@ -697,15 +697,15 @@
         <v>0.1</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2">
         <v>108</v>
@@ -714,15 +714,15 @@
         <v>0.13</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -731,15 +731,15 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
       </c>
       <c r="C12" s="2">
         <v>86</v>
@@ -748,15 +748,15 @@
         <v>0.1</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2">
         <v>9</v>
@@ -765,15 +765,15 @@
         <v>0.21</v>
       </c>
       <c r="G13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2">
         <v>36</v>
@@ -782,15 +782,15 @@
         <v>0.38</v>
       </c>
       <c r="G14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed voltage bug and added manufacturer column to output file
</commit_message>
<xml_diff>
--- a/BOMs/BOM_1.xlsx
+++ b/BOMs/BOM_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsheb\PushPin\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A00C3E6-521A-4469-A267-81CFF47E15F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799EA71E-A711-4606-807D-89DF04A4038D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4116" yWindow="156" windowWidth="17280" windowHeight="9960" xr2:uid="{D334EC07-162C-4D88-B7CF-9AC4FDBCC14E}"/>
+    <workbookView xWindow="4812" yWindow="852" windowWidth="17280" windowHeight="9960" xr2:uid="{D334EC07-162C-4D88-B7CF-9AC4FDBCC14E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Part Number</t>
   </si>
@@ -47,15 +47,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Manufactuer</t>
-  </si>
-  <si>
-    <t>AVX</t>
-  </si>
-  <si>
-    <t>Bourns</t>
-  </si>
-  <si>
     <t>CRM1206-JZ-3657ELF</t>
   </si>
   <si>
@@ -71,33 +62,21 @@
     <t>C10-C121</t>
   </si>
   <si>
-    <t>Darfon</t>
-  </si>
-  <si>
     <t>FRC32C1J599JB</t>
   </si>
   <si>
-    <t>Kamaya</t>
-  </si>
-  <si>
     <t>C1210C321K5PACTU</t>
   </si>
   <si>
     <t>C205-C209</t>
   </si>
   <si>
-    <t>Kemet</t>
-  </si>
-  <si>
     <t>C0201C100M9PACTU</t>
   </si>
   <si>
     <t>RK73H2HAGTE2726D</t>
   </si>
   <si>
-    <t>KOA</t>
-  </si>
-  <si>
     <t>RK73H1JATTD9R90F</t>
   </si>
   <si>
@@ -107,9 +86,6 @@
     <t>C210-C223</t>
   </si>
   <si>
-    <t>Meritek</t>
-  </si>
-  <si>
     <t>R37-R136</t>
   </si>
   <si>
@@ -119,9 +95,6 @@
     <t>C224-C244</t>
   </si>
   <si>
-    <t>Susumu</t>
-  </si>
-  <si>
     <t>R162-R269</t>
   </si>
   <si>
@@ -131,12 +104,6 @@
     <t>C245</t>
   </si>
   <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
     <t>RC0805JKP135K31L</t>
   </si>
   <si>
@@ -146,28 +113,16 @@
     <t>Unit Price</t>
   </si>
   <si>
-    <t>Expected Output</t>
-  </si>
-  <si>
     <t>GHOIJOIEFCNFJ32324</t>
   </si>
   <si>
     <t>U1-U4</t>
   </si>
   <si>
-    <t>UNKOWN</t>
-  </si>
-  <si>
     <t>R1-R43</t>
   </si>
   <si>
     <t>RR0816P-721-D</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>RK73H1ETTPE1R13F</t>
   </si>
   <si>
     <t>KAM15GS71C568CU</t>
@@ -531,7 +486,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,21 +510,17 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2">
         <v>84</v>
@@ -577,16 +528,13 @@
       <c r="D2" s="2">
         <v>0.31</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
         <v>112</v>
@@ -594,16 +542,13 @@
       <c r="D3" s="2">
         <v>0.2</v>
       </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
@@ -611,16 +556,13 @@
       <c r="D4" s="2">
         <v>0.1</v>
       </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2">
         <v>100</v>
@@ -628,16 +570,13 @@
       <c r="D5" s="2">
         <v>0.1</v>
       </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -645,16 +584,13 @@
       <c r="D6" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2">
         <v>14</v>
@@ -662,16 +598,13 @@
       <c r="D7" s="2">
         <v>0.24</v>
       </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2">
         <v>25</v>
@@ -679,16 +612,13 @@
       <c r="D8" s="2">
         <v>0.1</v>
       </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2">
         <v>21</v>
@@ -696,16 +626,13 @@
       <c r="D9" s="2">
         <v>0.1</v>
       </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2">
         <v>108</v>
@@ -713,16 +640,13 @@
       <c r="D10" s="2">
         <v>0.13</v>
       </c>
-      <c r="G10" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -730,16 +654,13 @@
       <c r="D11" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G11" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2">
         <v>86</v>
@@ -747,16 +668,13 @@
       <c r="D12" s="2">
         <v>0.1</v>
       </c>
-      <c r="G12" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2">
         <v>9</v>
@@ -764,16 +682,13 @@
       <c r="D13" s="2">
         <v>0.21</v>
       </c>
-      <c r="G13" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2">
         <v>36</v>
@@ -781,18 +696,8 @@
       <c r="D14" s="2">
         <v>0.38</v>
       </c>
-      <c r="G14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-    </row>
+    </row>
+    <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>